<commit_message>
Add R code for annual meeting plots
</commit_message>
<xml_diff>
--- a/2024/data/status.xlsx
+++ b/2024/data/status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,20 +71,20 @@
     <t>LL BET Index</t>
   </si>
   <si>
+    <t>LL BET LF</t>
+  </si>
+  <si>
+    <t>LL YFT Index</t>
+  </si>
+  <si>
     <t>LL YFT LF</t>
-  </si>
-  <si>
-    <t>LL BET LF</t>
-  </si>
-  <si>
-    <t>LL YFT Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,12 +431,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,75 +444,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
       </c>
       <c r="B13" s="2"/>
     </row>

</xml_diff>